<commit_message>
Challenge - Conditional Statement
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414BC15-727C-4042-B0D6-EEF0C16B3086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DFC0CB-B894-4849-B4C1-C20FF201A1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
     <sheet name="Switch-When Statement" sheetId="2" r:id="rId2"/>
+    <sheet name="Challenge-Conditional Statement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>構成</t>
   </si>
@@ -131,6 +132,84 @@
   </si>
   <si>
     <t xml:space="preserve">        System.debug('Good Evening');</t>
+  </si>
+  <si>
+    <t>Là 1 trong các giá trị 0,1,2,3,4,5,6,7,8,9,10,11 thì là "Good Morning"</t>
+  </si>
+  <si>
+    <t>Là 1 trong các giá trị 12,13,14,15,16 thì là "Good Afternoon"</t>
+  </si>
+  <si>
+    <t>3.leap-year-challenge-solution.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\3.leap-year-challenge-solution.txt</t>
+  </si>
+  <si>
+    <t>Năm nhuận</t>
+  </si>
+  <si>
+    <t>/*</t>
+  </si>
+  <si>
+    <t>&gt; A year is a leap year, if it is evenly divisible by 4.</t>
+  </si>
+  <si>
+    <t>&gt; Except if that is year is also evenly divisible by 100.</t>
+  </si>
+  <si>
+    <t>&gt; Unless the year is also evenly divisible by 400.</t>
+  </si>
+  <si>
+    <t>*/</t>
+  </si>
+  <si>
+    <t>Integer year = 2200;</t>
+  </si>
+  <si>
+    <t>// check if year is evenly divisible by 4</t>
+  </si>
+  <si>
+    <t>if(Math.mod(year, 4) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //check if year is evenly divisible by 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(Math.mod(year, 100) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // check if year is evenly divisible by 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if(Math.mod(year, 400) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug('Its a leap year');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        } else{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug('Not a leap year');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    } else{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        System.debug('Its a leap year');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    System.debug('Not a leap year');</t>
+  </si>
+  <si>
+    <t>Math.mod() để chia lấy phần dư</t>
+  </si>
+  <si>
+    <t>Chia hết cho 4 nhưng cũng chia hết cho 100 và ko chia hết cho 400 nên nó ko phải năm nhuận</t>
   </si>
 </sst>
 </file>
@@ -547,6 +626,152 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>156119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BEFCAF-F314-96DC-678F-D06A2AD8B5D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="647700"/>
+          <a:ext cx="11315700" cy="4461419"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>66961</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88DDD8B7-EE5D-A054-3980-195A5CCE1C1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="12477750"/>
+          <a:ext cx="11344275" cy="4924711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E59650F8-BE4B-1A7D-9829-6EF7CE13973E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3095625" y="8934450"/>
+          <a:ext cx="6134100" cy="4962525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -992,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E833685-1200-4F30-9162-ED07A7A4A674}">
   <dimension ref="A3:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,14 +1248,14 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
-      <c r="D7" s="11" t="s">
+      <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="6"/>
@@ -1077,164 +1302,101 @@
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
       <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
       <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>20</v>
       </c>
@@ -1249,4 +1411,344 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BBC922-2194-4C25-8E66-A692F98D06F4}">
+  <dimension ref="A3:J64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="D35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="D36" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="6"/>
+      <c r="H47" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="6"/>
+      <c r="H50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Loops In Apex - Do-While Loop
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DFC0CB-B894-4849-B4C1-C20FF201A1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E8C213-4EFE-441B-AF4E-37CAB4F84202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
     <sheet name="Switch-When Statement" sheetId="2" r:id="rId2"/>
     <sheet name="Challenge-Conditional Statement" sheetId="3" r:id="rId3"/>
+    <sheet name="Do-While Loop" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
   <si>
     <t>構成</t>
   </si>
@@ -210,6 +211,84 @@
   </si>
   <si>
     <t>Chia hết cho 4 nhưng cũng chia hết cho 100 và ko chia hết cho 400 nên nó ko phải năm nhuận</t>
+  </si>
+  <si>
+    <t>4.do-while-loop.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\4.do-while-loop.txt</t>
+  </si>
+  <si>
+    <t>// Print all leap years from year 1100 to year 2000</t>
+  </si>
+  <si>
+    <t>Integer year = 1100;</t>
+  </si>
+  <si>
+    <t>do {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //System.debug('Processing year '+year);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>// loop code block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // check if year is leap year or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // check if year is evenly divisible by 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(Math.mod(year, 4) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        //check if year is evenly divisible by 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if(Math.mod(year, 100) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            // check if year is evenly divisible by 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if(Math.mod(year, 400) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                System.debug(year + ' is a leap year');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug(year + ' is a leap year');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // increment year value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    year++;</t>
+  </si>
+  <si>
+    <t>} while(year &lt;= 2000);// year value must less than or equal to 2000</t>
+  </si>
+  <si>
+    <t>System.debug('Year value after loop '+ year);</t>
+  </si>
+  <si>
+    <t>Vòng lặp do-while: logic trong vòng lặp sẽ được execute ít nhất 1 lần</t>
+  </si>
+  <si>
+    <t>logic trong vòng lặp do-while sẽ được execute ít nhất 1 lần nên nếu khởi tạo year=2200 đã lớn hơn 2000</t>
+  </si>
+  <si>
+    <t>thì logic trong vòng lặp vẫn được thực hiện 1 lần đầu tiên</t>
+  </si>
+  <si>
+    <t>Giá trị của year sau khi kết thúc vòng lặp do-while</t>
   </si>
 </sst>
 </file>
@@ -772,6 +851,214 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>25633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4666611F-99A9-667F-A260-0F9D5DB828C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="9620251"/>
+          <a:ext cx="11268075" cy="4883382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBB0861E-D61E-7A92-EBBB-3145A235C99A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1790700" y="4914900"/>
+          <a:ext cx="10106025" cy="4095750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC9D8EBA-4A03-5C45-8978-34968EA0421D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="857250" y="5114925"/>
+          <a:ext cx="5486400" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D92EEBD-B374-52BD-9B68-8BABA412EEF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4029075" y="9496425"/>
+          <a:ext cx="2762250" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1417,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BBC922-2194-4C25-8E66-A692F98D06F4}">
   <dimension ref="A3:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1754,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
-      <c r="D35" s="11" t="s">
+      <c r="D35" t="s">
         <v>21</v>
       </c>
       <c r="H35" s="6"/>
@@ -1513,58 +1800,34 @@
       <c r="B42" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
       <c r="G42" s="6"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
       <c r="G43" s="6"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
       <c r="G44" s="6"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
       <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
       <c r="G46" s="6"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
       <c r="G47" s="6"/>
       <c r="H47" t="s">
         <v>6</v>
@@ -1575,30 +1838,18 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
       <c r="G48" s="6"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
       <c r="G49" s="6"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
       <c r="G50" s="6"/>
       <c r="H50" t="s">
         <v>6</v>
@@ -1611,130 +1862,78 @@
       <c r="B51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
       <c r="G51" s="6"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
       <c r="G52" s="6"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
       <c r="G53" s="6"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
       <c r="G54" s="6"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
       <c r="G55" s="6"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
       <c r="G56" s="6"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
       <c r="G57" s="6"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
       <c r="G58" s="6"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
       <c r="G59" s="6"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
       <c r="G60" s="6"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
       <c r="G62" s="6"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
@@ -1751,4 +1950,514 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0022F7B-D500-4AAF-9368-DCEF6CEB6AB0}">
+  <dimension ref="A2:K50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="D11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="D12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="6"/>
+      <c r="J26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="6"/>
+      <c r="K27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="10"/>
+      <c r="J50" t="s">
+        <v>6</v>
+      </c>
+      <c r="K50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Challenge - Do-While Loop
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E8C213-4EFE-441B-AF4E-37CAB4F84202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3240666-4AE4-433E-9670-0B8012DE1A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
     <sheet name="Switch-When Statement" sheetId="2" r:id="rId2"/>
     <sheet name="Challenge-Conditional Statement" sheetId="3" r:id="rId3"/>
     <sheet name="Do-While Loop" sheetId="4" r:id="rId4"/>
+    <sheet name="Challenge - Do-While Loop" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="106">
   <si>
     <t>構成</t>
   </si>
@@ -285,10 +286,67 @@
     <t>logic trong vòng lặp do-while sẽ được execute ít nhất 1 lần nên nếu khởi tạo year=2200 đã lớn hơn 2000</t>
   </si>
   <si>
-    <t>thì logic trong vòng lặp vẫn được thực hiện 1 lần đầu tiên</t>
-  </si>
-  <si>
     <t>Giá trị của year sau khi kết thúc vòng lặp do-while</t>
+  </si>
+  <si>
+    <t>5.do-while-challenge-solution.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\5.do-while-challenge-solution.txt</t>
+  </si>
+  <si>
+    <t>Integer i = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // check if i is divisible by both 3 and 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(Math.mod(i, 3) == 0 &amp;&amp; Math.mod(i, 5) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        System.debug('fizzbuzz');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    } else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        //check if i is divisible by 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if(Math.mod(i, 3) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug('fizz');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        //check if i is divisible by 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        else if(Math.mod(i, 5) == 0){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug('buzz');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // if none of above is true, then print i as is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug(i);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // increment i's value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    i++;</t>
+  </si>
+  <si>
+    <t>} while ( i&lt;=100);//i's value is less than or equal to 100</t>
+  </si>
+  <si>
+    <t>thì logic trong vòng lặp vẫn được thực hiện 1 lần đầu tiên và year sau vòng lặp sẽ là 2201</t>
   </si>
 </sst>
 </file>
@@ -1056,6 +1114,152 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD7483AA-A75C-1131-97C4-C3C27331FBFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3152775" y="5086350"/>
+          <a:ext cx="7829550" cy="4314825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>102317</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6484A044-7016-D0EE-53C9-F441DC9FE198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="457201"/>
+          <a:ext cx="11306175" cy="4026616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>123364</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE3364A1-E4E8-CCA9-02B3-F985FCD6439A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="12449175"/>
+          <a:ext cx="11258550" cy="4819189"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1956,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0022F7B-D500-4AAF-9368-DCEF6CEB6AB0}">
   <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2217,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="D11" s="11" t="s">
+      <c r="D11" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="6"/>
@@ -2061,102 +2265,48 @@
       <c r="B18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
       <c r="I26" s="6"/>
       <c r="J26" t="s">
         <v>6</v>
@@ -2167,275 +2317,138 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
       <c r="I27" s="6"/>
       <c r="K27" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2453,8 +2466,369 @@
         <v>6</v>
       </c>
       <c r="K50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30541B4-C6CA-4375-BA4F-A9A139C90882}">
+  <dimension ref="A27:J63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="D34" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="D35" s="7" t="s">
         <v>86</v>
       </c>
+      <c r="H35" s="6"/>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="5"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Challenge - While Loop
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29738170-F658-490A-8D2A-E904AC3C000F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FAD6F1-DBFA-442C-9B27-E63ECB44D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Do-While Loop" sheetId="4" r:id="rId4"/>
     <sheet name="Challenge - Do-While Loop" sheetId="5" r:id="rId5"/>
     <sheet name="While Loop" sheetId="6" r:id="rId6"/>
+    <sheet name="Challenge - While Loop" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="143">
   <si>
     <t>構成</t>
   </si>
@@ -366,6 +367,99 @@
   </si>
   <si>
     <t>Khác với do-while, nếu year được khởi tạo là 2200 lơn hơn 2000 nên logic sẽ ko được thực hiện bất cứ lần nào</t>
+  </si>
+  <si>
+    <t>In ra 20 số đầu trong dãy Fibonacci</t>
+  </si>
+  <si>
+    <t>7.while-loop-challege-solution.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\7.while-loop-challege-solution.txt</t>
+  </si>
+  <si>
+    <t>Print first 20 fibonacci numbers</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 2, 3, 5, 8 …</t>
+  </si>
+  <si>
+    <t>0 &amp; 1 - first 2 numbers</t>
+  </si>
+  <si>
+    <t>1 &gt; 0+1</t>
+  </si>
+  <si>
+    <t>2 &gt; 1+1</t>
+  </si>
+  <si>
+    <t>3 &gt; 2+1</t>
+  </si>
+  <si>
+    <t>5 &gt; 3+2</t>
+  </si>
+  <si>
+    <t>Integer current;</t>
+  </si>
+  <si>
+    <t>Integer previous = 1;</t>
+  </si>
+  <si>
+    <t>Integer beforePrevious = 0;</t>
+  </si>
+  <si>
+    <t>// current = previous + beforePrevious</t>
+  </si>
+  <si>
+    <t>// current = 1 + 0 = 1</t>
+  </si>
+  <si>
+    <t>// print very first number</t>
+  </si>
+  <si>
+    <t>System.debug(beforePrevious);</t>
+  </si>
+  <si>
+    <t>// print 2nd number</t>
+  </si>
+  <si>
+    <t>System.debug(previous);</t>
+  </si>
+  <si>
+    <t>// print next 18 numbers</t>
+  </si>
+  <si>
+    <t>while(i&lt;18){//run loop 18 times</t>
+  </si>
+  <si>
+    <t>//print fibonacci numbers here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //calculate current number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    current = previous + beforePrevious;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //print current value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    System.debug(current);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //update beforePrevious with previous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    beforePrevious = previous;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //update previous with current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    previous = current;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //increment i's value</t>
   </si>
 </sst>
 </file>
@@ -506,8 +600,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,6 +1478,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523136</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>65908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC4D8058-85D2-E4A2-2893-41E92809C480}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="600075"/>
+          <a:ext cx="5914286" cy="6133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>525169</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E813BEDE-E6F6-DA5E-505E-64D7E2D4EE4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="11620500"/>
+          <a:ext cx="13707769" cy="6219825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2851,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDBC82F-8483-4E2D-988A-0AD19729C5CF}">
   <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +3109,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="D13" s="11" t="s">
+      <c r="D13" t="s">
         <v>86</v>
       </c>
       <c r="H13" s="6"/>
@@ -2970,92 +3157,44 @@
       <c r="B20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
       <c r="I27" s="6"/>
       <c r="J27" t="s">
         <v>6</v>
@@ -3066,252 +3205,127 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
@@ -3330,4 +3344,964 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADABD43-6CF2-4C4A-B257-3EB3F80CA154}">
+  <dimension ref="A3:K94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I98" sqref="I98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="10"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="D44" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="D48" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="D49" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H49" s="6"/>
+      <c r="I49" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="10"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="5"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="6"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="6"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="6"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="6"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="6"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="C80" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="6"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="6"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="6"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="6"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="6"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="6"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="6"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="6"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="6"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Challenge - For Loop
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF46B8B-848E-4D59-BE9D-4F247A8F7C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F46BAB-3356-48FD-80B0-2F7FFC19B789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="While Loop" sheetId="6" r:id="rId6"/>
     <sheet name="Challenge - While Loop" sheetId="7" r:id="rId7"/>
     <sheet name="For Loop" sheetId="8" r:id="rId8"/>
+    <sheet name="Challenge - For Loop" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="165">
   <si>
     <t>構成</t>
   </si>
@@ -473,6 +474,60 @@
   </si>
   <si>
     <t>for(Integer year = 1100; year &lt;= 2000; year++){</t>
+  </si>
+  <si>
+    <t>9.for-loop-challenge-solution.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\9.for-loop-challenge-solution.txt</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>*   *</t>
+  </si>
+  <si>
+    <t>*   *   *</t>
+  </si>
+  <si>
+    <t>*   *   *   *</t>
+  </si>
+  <si>
+    <t>*   *   *   *   *</t>
+  </si>
+  <si>
+    <t>Integer n = 5;</t>
+  </si>
+  <si>
+    <t>// for loop to build rows</t>
+  </si>
+  <si>
+    <t>for(Integer row  = 0; row &lt; n; row++) {</t>
+  </si>
+  <si>
+    <t>String pattern = '';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //System.debug('*');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // for loop to build columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for(Integer column = 0; column &lt;= row; column++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        //System.debug('*');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        pattern = pattern + '*  '; // or pattern+='*  ';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    //print pattern here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    System.debug(pattern);</t>
   </si>
 </sst>
 </file>
@@ -1730,6 +1785,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>90142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FAC4609-01C0-0CB8-F93E-3C7D84E27876}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="8886825"/>
+          <a:ext cx="11172825" cy="4919317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4019,8 +4123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAB0C13-BC51-44B8-B977-9162C019AE21}">
   <dimension ref="A27:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4099,7 +4203,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="D37" s="11" t="s">
+      <c r="D37" t="s">
         <v>113</v>
       </c>
       <c r="H37" s="6"/>
@@ -4146,6 +4250,541 @@
       <c r="B44" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" t="s">
+        <v>68</v>
+      </c>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA77EB4-7CFF-4E87-BDD5-37B15EF2CA35}">
+  <dimension ref="A3:J45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="D11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="D13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="D14" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="D15" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -4153,267 +4792,16 @@
       <c r="G44" s="12"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="5"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="5"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="6"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="6"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="6"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="6"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="6"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="6"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="6"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="6"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="6"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="6"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="6"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="6"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="6"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="6"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="6"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="6"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="8" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="10"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Break Statement - Breaking a Loop
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F46BAB-3356-48FD-80B0-2F7FFC19B789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1790FD1D-49A4-44BC-953B-00EC4CC788A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Challenge - While Loop" sheetId="7" r:id="rId7"/>
     <sheet name="For Loop" sheetId="8" r:id="rId8"/>
     <sheet name="Challenge - For Loop" sheetId="9" r:id="rId9"/>
+    <sheet name="Break Statement" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="177">
   <si>
     <t>構成</t>
   </si>
@@ -528,6 +529,42 @@
   </si>
   <si>
     <t xml:space="preserve">    System.debug(pattern);</t>
+  </si>
+  <si>
+    <t>10.break-statement.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\10.break-statement.txt</t>
+  </si>
+  <si>
+    <t>// get goosebumps after listening to the song  these many time</t>
+  </si>
+  <si>
+    <t>Integer gooseBumpsAfter = 4;</t>
+  </si>
+  <si>
+    <t>// Iterate over the map for a maximum 1000 times</t>
+  </si>
+  <si>
+    <t>Integer n = 1000;</t>
+  </si>
+  <si>
+    <t>for(Integer i=1; i&lt;=n; i++){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    System.debug('Listening to song ' + i + ' times');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // break the loop if i equals to gooseBumpsAfter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(i == gooseBumpsAfter){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        break;</t>
+  </si>
+  <si>
+    <t>Dùng break để thoát ra khỏi vòng lặp và ko cần thực hiện các vòng lặp tiếp theo nữa</t>
   </si>
 </sst>
 </file>
@@ -656,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -668,7 +705,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -784,6 +830,55 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>117535</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FBCFADB-890A-C79C-D5EE-37000294FC71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="7143750"/>
+          <a:ext cx="11115675" cy="4784785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2275,6 +2370,381 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E43605E-BD5C-45A2-A386-58294931FD1D}">
+  <dimension ref="A2:J35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E833685-1200-4F30-9162-ED07A7A4A674}">
   <dimension ref="A3:J29"/>
@@ -4410,8 +4880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA77EB4-7CFF-4E87-BDD5-37B15EF2CA35}">
   <dimension ref="A3:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4497,7 +4967,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" t="s">
         <v>143</v>
       </c>
       <c r="H14" s="6"/>
@@ -4542,254 +5012,135 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
-      <c r="C35" s="12" t="s">
+      <c r="C35" t="s">
         <v>157</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
       <c r="H43" s="6"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Continue Statement - Skipping Loop Iteration
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1790FD1D-49A4-44BC-953B-00EC4CC788A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF76AB20-F5FE-4567-8DFA-9198CA092937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="For Loop" sheetId="8" r:id="rId8"/>
     <sheet name="Challenge - For Loop" sheetId="9" r:id="rId9"/>
     <sheet name="Break Statement" sheetId="10" r:id="rId10"/>
+    <sheet name="Continue Statement" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="191">
   <si>
     <t>構成</t>
   </si>
@@ -565,6 +566,48 @@
   </si>
   <si>
     <t>Dùng break để thoát ra khỏi vòng lặp và ko cần thực hiện các vòng lặp tiếp theo nữa</t>
+  </si>
+  <si>
+    <t>Dùng continue để bỏ qua bước lặp hiện tại để nhẩy đến bước lặp tiếp theo</t>
+  </si>
+  <si>
+    <t>11.continue-statement.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\11.continue-statement.txt</t>
+  </si>
+  <si>
+    <t>//List of all days</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; days = new List&lt;String&gt;{'Monday','Tuesday','Wednesday','Thursday','Friday','Saturday','Sunday'};</t>
+  </si>
+  <si>
+    <t>// get the list size</t>
+  </si>
+  <si>
+    <t>Integer listSize = days.size();</t>
+  </si>
+  <si>
+    <t>//iterate over the list</t>
+  </si>
+  <si>
+    <t>for(Integer i=0; i &lt; listSize; i++){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(days.get(i) == 'Tuesday'){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        continue;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    System.debug('It is '+days.get(i)+'. Eat Chicken.');</t>
+  </si>
+  <si>
+    <t>Nếu là 'Tuesday' thì ko thực hiện gì ở bước lặp này nữa mà nhảy đến bước lặp</t>
+  </si>
+  <si>
+    <t>tiếp theo</t>
   </si>
 </sst>
 </file>
@@ -693,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -705,16 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -873,6 +907,55 @@
         <a:xfrm>
           <a:off x="695325" y="7143750"/>
           <a:ext cx="11115675" cy="4784785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>32448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{533BA2F9-AF6E-180F-EE01-DE15E98D1CD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="7334250"/>
+          <a:ext cx="11125200" cy="4890198"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2374,226 +2457,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E43605E-BD5C-45A2-A386-58294931FD1D}">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="12" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="12" t="s">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12" t="s">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12" t="s">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12" t="s">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="D14" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="D15" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12" t="s">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="D16" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12" t="s">
+      <c r="B17" s="5"/>
+      <c r="D17" t="s">
         <v>147</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="5"/>
       <c r="D18" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="12" t="s">
+      <c r="H18" s="6"/>
+      <c r="I18" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2615,117 +2603,62 @@
       <c r="B24" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -2738,6 +2671,354 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDFC049-6541-4987-9191-1C71D232C973}">
+  <dimension ref="A2:N36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="D15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="D16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="D17" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="D18" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="D19" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="6"/>
+      <c r="M32" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="6"/>
+      <c r="N33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
List Iteration For Loops
</commit_message>
<xml_diff>
--- a/me/3.Control-Flow-Statements.xlsx
+++ b/me/3.Control-Flow-Statements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF76AB20-F5FE-4567-8DFA-9198CA092937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A72930E-DFC8-4AF3-BC9F-FA3DF18F3797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If-Else Statement" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Challenge - For Loop" sheetId="9" r:id="rId9"/>
     <sheet name="Break Statement" sheetId="10" r:id="rId10"/>
     <sheet name="Continue Statement" sheetId="11" r:id="rId11"/>
+    <sheet name="List Iteration For Loops" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="200">
   <si>
     <t>構成</t>
   </si>
@@ -608,6 +609,33 @@
   </si>
   <si>
     <t>tiếp theo</t>
+  </si>
+  <si>
+    <t>List/Set Iteration For Loops</t>
+  </si>
+  <si>
+    <t>Lặp tất cả các item trong List hoặc Set, nó cũng được gọi là vòng lặp for nhưng nó giúp lặp các item trong List và Set 1 cách dễ dàng</t>
+  </si>
+  <si>
+    <t>12.list-iteration-for-loop.txt</t>
+  </si>
+  <si>
+    <t>salesforce\3.Control-Flow-Statements\12.list-iteration-for-loop.txt</t>
+  </si>
+  <si>
+    <t>// list iteration for loop to iterate over days</t>
+  </si>
+  <si>
+    <t>for(String day : days){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(day == 'Tuesday'){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    System.debug('It is '+day+'. Eat Chicken');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -736,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -748,7 +776,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -956,6 +993,55 @@
         <a:xfrm>
           <a:off x="695325" y="7334250"/>
           <a:ext cx="11125200" cy="4890198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>47911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB165600-A7C7-B3FE-2C8B-027D88ADAD8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="7124700"/>
+          <a:ext cx="11344275" cy="4924711"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2682,8 +2768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDFC049-6541-4987-9191-1C71D232C973}">
   <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2874,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="D18" s="11" t="s">
+      <c r="D18" t="s">
         <v>165</v>
       </c>
       <c r="H18" s="6"/>
@@ -2839,116 +2925,44 @@
       <c r="B25" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
       <c r="L32" s="6"/>
       <c r="M32" t="s">
         <v>6</v>
@@ -2961,15 +2975,6 @@
       <c r="B33" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
       <c r="L33" s="6"/>
       <c r="N33" t="s">
         <v>190</v>
@@ -2979,30 +2984,12 @@
       <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
       <c r="L34" s="6"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
       <c r="L35" s="6"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -3019,6 +3006,428 @@
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FEFB26-D1C7-4698-AAC9-380B80F8B5F3}">
+  <dimension ref="A2:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="10"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>199</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>